<commit_message>
Alterei as cores no relatorio
</commit_message>
<xml_diff>
--- a/Relatório/Relatório gráfico.xlsx
+++ b/Relatório/Relatório gráfico.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitoria\Documents\Bandtec\Pesquisa e inovação\Projeto-P-I\Projeto-P-I\Relatório\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\Projeto Sprint 2\Projeto-P-I\Relatório\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE448D2D-A58B-43BA-AA41-4AC37BDAA68B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CACFC0-5E75-4CAA-8E3B-CA1FE8051694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -185,20 +188,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,20 +277,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -303,8 +295,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -461,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -499,10 +521,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -510,9 +528,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -533,41 +571,42 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3562,54 +3601,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F1:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V4" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.7109375" customWidth="1"/>
-    <col min="37" max="37" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.5703125" customWidth="1"/>
-    <col min="41" max="41" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" customWidth="1"/>
+    <col min="37" max="37" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.5546875" customWidth="1"/>
+    <col min="41" max="41" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:41" x14ac:dyDescent="0.25">
-      <c r="F1" s="30" t="s">
+    <row r="1" spans="6:41" x14ac:dyDescent="0.3">
+      <c r="F1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="AD1" s="29" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="AD1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
     </row>
-    <row r="2" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
@@ -3629,7 +3668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F3" s="8">
         <v>1</v>
       </c>
@@ -3639,25 +3678,25 @@
       <c r="H3" s="14">
         <v>62</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
       <c r="AD3" s="7">
         <v>1</v>
       </c>
-      <c r="AE3" s="22">
+      <c r="AE3" s="20">
         <v>22</v>
       </c>
-      <c r="AF3" s="23">
+      <c r="AF3" s="20">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F4" s="8">
         <v>2</v>
       </c>
@@ -3688,14 +3727,14 @@
       <c r="AD4" s="7">
         <v>2</v>
       </c>
-      <c r="AE4" s="22">
+      <c r="AE4" s="20">
         <v>21</v>
       </c>
-      <c r="AF4" s="24">
+      <c r="AF4" s="61">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F5" s="8">
         <v>3</v>
       </c>
@@ -3705,59 +3744,59 @@
       <c r="H5" s="14">
         <v>64</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="41">
         <f>MIN(G3:G32)</f>
         <v>12</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="44">
         <f>_xlfn.QUARTILE.EXC(G3:G32,1)</f>
         <v>19</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="50">
         <f>AVERAGE(G3:G32)</f>
         <v>23.366666666666667</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="44">
         <f>MEDIAN(G3:G32)</f>
         <v>24</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="44">
         <f>_xlfn.QUARTILE.EXC(G3:G32,3)</f>
         <v>26.5</v>
       </c>
-      <c r="O5" s="41">
+      <c r="O5" s="45">
         <f>MAX(G3:G32)</f>
         <v>35</v>
       </c>
-      <c r="R5" s="37" t="s">
+      <c r="R5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
       <c r="AD5" s="7">
         <v>3</v>
       </c>
-      <c r="AE5" s="22">
+      <c r="AE5" s="20">
         <v>22</v>
       </c>
-      <c r="AF5" s="23">
+      <c r="AF5" s="62">
         <v>65</v>
       </c>
-      <c r="AJ5" s="29" t="s">
+      <c r="AJ5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="AK5" s="29"/>
-      <c r="AL5" s="29"/>
-      <c r="AM5" s="29"/>
-      <c r="AN5" s="29"/>
-      <c r="AO5" s="29"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="35"/>
+      <c r="AM5" s="35"/>
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="35"/>
     </row>
-    <row r="6" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F6" s="8">
         <v>4</v>
       </c>
@@ -3767,53 +3806,53 @@
       <c r="H6" s="14">
         <v>61</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="34"/>
-      <c r="R6" s="35" t="s">
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="40"/>
+      <c r="R6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
       <c r="AD6" s="7">
         <v>4</v>
       </c>
-      <c r="AE6" s="22">
+      <c r="AE6" s="20">
         <v>24</v>
       </c>
-      <c r="AF6" s="23">
+      <c r="AF6" s="20">
         <v>66</v>
       </c>
-      <c r="AJ6" s="49" t="s">
+      <c r="AJ6" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="AK6" s="49" t="s">
+      <c r="AK6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="AL6" s="48" t="s">
+      <c r="AL6" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="AM6" s="48" t="s">
+      <c r="AM6" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="AN6" s="27" t="s">
+      <c r="AN6" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AO6" s="26" t="s">
+      <c r="AO6" s="54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F7" s="8">
         <v>5</v>
       </c>
@@ -3841,65 +3880,65 @@
       <c r="O7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="4" t="s">
+      <c r="U7" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="4" t="s">
+      <c r="V7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="X7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Y7" s="49" t="s">
         <v>10</v>
       </c>
       <c r="AD7" s="7">
         <v>5</v>
       </c>
-      <c r="AE7" s="22">
+      <c r="AE7" s="20">
         <v>23</v>
       </c>
-      <c r="AF7" s="23">
+      <c r="AF7" s="20">
         <v>67</v>
       </c>
-      <c r="AJ7" s="49">
+      <c r="AJ7" s="28">
         <f>MIN(AE3:AE32)</f>
         <v>21</v>
       </c>
-      <c r="AK7" s="49">
+      <c r="AK7" s="28">
         <f>_xlfn.QUARTILE.EXC(AE3:AE32,1)</f>
         <v>23</v>
       </c>
-      <c r="AL7" s="48">
+      <c r="AL7" s="27">
         <f>AVERAGE(AE3:AE32)</f>
         <v>26.5</v>
       </c>
-      <c r="AM7" s="48">
+      <c r="AM7" s="27">
         <f>MEDIAN(AE3:AE32)</f>
         <v>25</v>
       </c>
-      <c r="AN7" s="27">
+      <c r="AN7" s="24">
         <f>_xlfn.QUARTILE.EXC(AE3:AE32,3)</f>
         <v>30.25</v>
       </c>
-      <c r="AO7" s="42">
+      <c r="AO7" s="25">
         <f>MAX(AE3:AE32)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F8" s="8">
         <v>6</v>
       </c>
@@ -3909,27 +3948,27 @@
       <c r="H8" s="14">
         <v>54</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="41">
         <f>MIN(H3:H32)</f>
         <v>39</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="17">
         <f>_xlfn.QUARTILE.EXC(H3:H32,1)</f>
         <v>50.75</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="18">
         <f>AVERAGE(H3:H32)</f>
         <v>58.233333333333334</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="17">
         <f>MEDIAN(H3:H32)</f>
         <v>61.5</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="17">
         <f>_xlfn.QUARTILE.EXC(H3:H32,3)</f>
         <v>64</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="19">
         <f>MAX(H3:H32)</f>
         <v>74</v>
       </c>
@@ -3960,14 +3999,14 @@
       <c r="AD8" s="7">
         <v>6</v>
       </c>
-      <c r="AE8" s="22">
+      <c r="AE8" s="20">
         <v>25</v>
       </c>
-      <c r="AF8" s="24">
+      <c r="AF8" s="62">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F9" s="8">
         <v>7</v>
       </c>
@@ -3980,72 +4019,72 @@
       <c r="AD9" s="7">
         <v>7</v>
       </c>
-      <c r="AE9" s="22">
+      <c r="AE9" s="20">
         <v>23</v>
       </c>
-      <c r="AF9" s="24">
+      <c r="AF9" s="62">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F10" s="8">
         <v>8</v>
       </c>
       <c r="G10" s="15">
         <v>30</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="51">
         <v>46</v>
       </c>
       <c r="J10" s="11"/>
-      <c r="R10" s="36" t="s">
+      <c r="R10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="36"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
       <c r="AD10" s="7">
         <v>8</v>
       </c>
-      <c r="AE10" s="22">
+      <c r="AE10" s="20">
         <v>24</v>
       </c>
-      <c r="AF10" s="24">
+      <c r="AF10" s="62">
         <v>63</v>
       </c>
-      <c r="AJ10" s="29" t="s">
+      <c r="AJ10" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AK10" s="29"/>
-      <c r="AL10" s="29"/>
-      <c r="AM10" s="29"/>
-      <c r="AN10" s="29"/>
-      <c r="AO10" s="29"/>
+      <c r="AK10" s="35"/>
+      <c r="AL10" s="35"/>
+      <c r="AM10" s="35"/>
+      <c r="AN10" s="35"/>
+      <c r="AO10" s="35"/>
     </row>
-    <row r="11" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F11" s="8">
         <v>9</v>
       </c>
       <c r="G11" s="14">
         <v>28</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="52">
         <v>43</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="S11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T11" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="U11" s="4" t="s">
+      <c r="U11" s="44" t="s">
         <v>13</v>
       </c>
       <c r="V11" s="4" t="s">
@@ -4063,39 +4102,39 @@
       <c r="AD11" s="7">
         <v>9</v>
       </c>
-      <c r="AE11" s="22">
+      <c r="AE11" s="20">
         <v>21</v>
       </c>
-      <c r="AF11" s="23">
+      <c r="AF11" s="20">
         <v>66</v>
       </c>
-      <c r="AJ11" s="42" t="s">
+      <c r="AJ11" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="AK11" s="42" t="s">
+      <c r="AK11" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="AL11" s="44" t="s">
+      <c r="AL11" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="AM11" s="44" t="s">
+      <c r="AM11" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="AN11" s="27" t="s">
+      <c r="AN11" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="AO11" s="26" t="s">
+      <c r="AO11" s="54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F12" s="8">
         <v>10</v>
       </c>
       <c r="G12" s="14">
         <v>23</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="53">
         <v>39</v>
       </c>
       <c r="R12" s="5">
@@ -4125,157 +4164,157 @@
       <c r="AD12" s="7">
         <v>10</v>
       </c>
-      <c r="AE12" s="22">
+      <c r="AE12" s="20">
         <v>26</v>
       </c>
-      <c r="AF12" s="24">
+      <c r="AF12" s="62">
         <v>61</v>
       </c>
-      <c r="AJ12" s="47">
+      <c r="AJ12" s="56">
         <f>MIN(AF3:AF32)</f>
         <v>44</v>
       </c>
-      <c r="AK12" s="47">
+      <c r="AK12" s="56">
         <f>_xlfn.QUARTILE.EXC(AF3:AF32,1)</f>
         <v>54</v>
       </c>
-      <c r="AL12" s="45">
+      <c r="AL12" s="57">
         <f>AVERAGE(AF3:AF32)</f>
         <v>58.366666666666667</v>
       </c>
-      <c r="AM12" s="46">
+      <c r="AM12" s="58">
         <f>MEDIAN(AF3:AF32)</f>
         <v>58.5</v>
       </c>
-      <c r="AN12" s="28">
+      <c r="AN12" s="59">
         <f>_xlfn.QUARTILE.EXC(AF3:AF32,3)</f>
         <v>64</v>
       </c>
-      <c r="AO12" s="43">
+      <c r="AO12" s="26">
         <f>MAX(AF3:AF32)</f>
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F13" s="8">
         <v>11</v>
       </c>
       <c r="G13" s="14">
         <v>19</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="52">
         <v>44</v>
       </c>
       <c r="AD13" s="7">
         <v>11</v>
       </c>
-      <c r="AE13" s="22">
+      <c r="AE13" s="20">
         <v>25</v>
       </c>
-      <c r="AF13" s="24">
+      <c r="AF13" s="62">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F14" s="8">
         <v>12</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="51">
         <v>16</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="14">
         <v>49</v>
       </c>
       <c r="AD14" s="7">
         <v>12</v>
       </c>
-      <c r="AE14" s="22">
+      <c r="AE14" s="20">
         <v>24</v>
       </c>
-      <c r="AF14" s="23">
+      <c r="AF14" s="62">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F15" s="8">
         <v>13</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="52">
         <v>13</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="51">
         <v>47</v>
       </c>
-      <c r="R15" s="38" t="s">
+      <c r="R15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="S15" s="39"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="39"/>
-      <c r="V15" s="39"/>
-      <c r="W15" s="39"/>
-      <c r="X15" s="39"/>
-      <c r="Y15" s="40"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="34"/>
       <c r="AD15" s="7">
         <v>13</v>
       </c>
-      <c r="AE15" s="22">
+      <c r="AE15" s="20">
         <v>23</v>
       </c>
-      <c r="AF15" s="24">
+      <c r="AF15" s="62">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="6:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:41" x14ac:dyDescent="0.3">
       <c r="F16" s="8">
         <v>14</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="53">
         <v>12</v>
       </c>
       <c r="H16" s="14">
         <v>52</v>
       </c>
-      <c r="R16" s="35" t="s">
+      <c r="R16" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
       <c r="AD16" s="7">
         <v>14</v>
       </c>
-      <c r="AE16" s="22">
+      <c r="AE16" s="20">
         <v>22</v>
       </c>
-      <c r="AF16" s="24">
+      <c r="AF16" s="62">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F17" s="8">
         <v>15</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="52">
         <v>16</v>
       </c>
       <c r="H17" s="14">
         <v>51</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="R17" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="S17" s="3" t="s">
+      <c r="S17" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="T17" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="U17" s="4" t="s">
+      <c r="U17" s="44" t="s">
         <v>13</v>
       </c>
       <c r="V17" s="4" t="s">
@@ -4293,14 +4332,14 @@
       <c r="AD17" s="7">
         <v>15</v>
       </c>
-      <c r="AE17" s="22">
+      <c r="AE17" s="20">
         <v>21</v>
       </c>
-      <c r="AF17" s="25">
+      <c r="AF17" s="61">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F18" s="8">
         <v>16</v>
       </c>
@@ -4337,14 +4376,14 @@
       <c r="AD18" s="7">
         <v>16</v>
       </c>
-      <c r="AE18" s="22">
+      <c r="AE18" s="20">
         <v>26</v>
       </c>
-      <c r="AF18" s="25">
+      <c r="AF18" s="61">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F19" s="8">
         <v>17</v>
       </c>
@@ -4357,14 +4396,14 @@
       <c r="AD19" s="7">
         <v>17</v>
       </c>
-      <c r="AE19" s="22">
+      <c r="AE19" s="20">
         <v>24</v>
       </c>
-      <c r="AF19" s="25">
+      <c r="AF19" s="61">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F20" s="8">
         <v>18</v>
       </c>
@@ -4374,27 +4413,27 @@
       <c r="H20" s="14">
         <v>64</v>
       </c>
-      <c r="R20" s="36" t="s">
+      <c r="R20" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="30"/>
       <c r="AD20" s="7">
         <v>18</v>
       </c>
-      <c r="AE20" s="22">
+      <c r="AE20" s="20">
         <v>23</v>
       </c>
-      <c r="AF20" s="25">
+      <c r="AF20" s="60">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F21" s="8">
         <v>19</v>
       </c>
@@ -4404,16 +4443,16 @@
       <c r="H21" s="14">
         <v>67</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="R21" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="S21" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="U21" s="4" t="s">
+      <c r="U21" s="44" t="s">
         <v>13</v>
       </c>
       <c r="V21" s="4" t="s">
@@ -4431,14 +4470,14 @@
       <c r="AD21" s="7">
         <v>19</v>
       </c>
-      <c r="AE21" s="22">
+      <c r="AE21" s="20">
         <v>27</v>
       </c>
-      <c r="AF21" s="25">
+      <c r="AF21" s="60">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F22" s="8">
         <v>20</v>
       </c>
@@ -4475,14 +4514,14 @@
       <c r="AD22" s="7">
         <v>20</v>
       </c>
-      <c r="AE22" s="22">
+      <c r="AE22" s="20">
         <v>28</v>
       </c>
-      <c r="AF22" s="25">
+      <c r="AF22" s="60">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F23" s="8">
         <v>21</v>
       </c>
@@ -4495,14 +4534,14 @@
       <c r="AD23" s="7">
         <v>21</v>
       </c>
-      <c r="AE23" s="22">
+      <c r="AE23" s="20">
         <v>27</v>
       </c>
-      <c r="AF23" s="25">
+      <c r="AF23" s="60">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F24" s="8">
         <v>22</v>
       </c>
@@ -4515,14 +4554,14 @@
       <c r="AD24" s="7">
         <v>22</v>
       </c>
-      <c r="AE24" s="23">
+      <c r="AE24" s="21">
         <v>29</v>
       </c>
-      <c r="AF24" s="25">
+      <c r="AF24" s="61">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F25" s="8">
         <v>23</v>
       </c>
@@ -4535,14 +4574,14 @@
       <c r="AD25" s="7">
         <v>23</v>
       </c>
-      <c r="AE25" s="23">
+      <c r="AE25" s="21">
         <v>30</v>
       </c>
-      <c r="AF25" s="25">
+      <c r="AF25" s="61">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F26" s="8">
         <v>24</v>
       </c>
@@ -4555,14 +4594,14 @@
       <c r="AD26" s="7">
         <v>24</v>
       </c>
-      <c r="AE26" s="24">
+      <c r="AE26" s="22">
         <v>31</v>
       </c>
-      <c r="AF26" s="25">
+      <c r="AF26" s="60">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F27" s="8">
         <v>25</v>
       </c>
@@ -4575,14 +4614,14 @@
       <c r="AD27" s="7">
         <v>25</v>
       </c>
-      <c r="AE27" s="24">
+      <c r="AE27" s="22">
         <v>31</v>
       </c>
-      <c r="AF27" s="25">
+      <c r="AF27" s="60">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F28" s="8">
         <v>26</v>
       </c>
@@ -4595,14 +4634,14 @@
       <c r="AD28" s="7">
         <v>26</v>
       </c>
-      <c r="AE28" s="24">
+      <c r="AE28" s="22">
         <v>32</v>
       </c>
-      <c r="AF28" s="25">
+      <c r="AF28" s="60">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F29" s="8">
         <v>27</v>
       </c>
@@ -4615,14 +4654,14 @@
       <c r="AD29" s="7">
         <v>27</v>
       </c>
-      <c r="AE29" s="25">
+      <c r="AE29" s="23">
         <v>36</v>
       </c>
-      <c r="AF29" s="25">
+      <c r="AF29" s="60">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F30" s="8">
         <v>28</v>
       </c>
@@ -4635,14 +4674,14 @@
       <c r="AD30" s="7">
         <v>28</v>
       </c>
-      <c r="AE30" s="24">
+      <c r="AE30" s="22">
         <v>33</v>
       </c>
-      <c r="AF30" s="25">
+      <c r="AF30" s="60">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F31" s="8">
         <v>29</v>
       </c>
@@ -4655,14 +4694,14 @@
       <c r="AD31" s="7">
         <v>29</v>
       </c>
-      <c r="AE31" s="25">
+      <c r="AE31" s="23">
         <v>35</v>
       </c>
-      <c r="AF31" s="25">
+      <c r="AF31" s="60">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="6:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:32" x14ac:dyDescent="0.3">
       <c r="F32" s="8">
         <v>30</v>
       </c>
@@ -4675,27 +4714,27 @@
       <c r="AD32" s="7">
         <v>30</v>
       </c>
-      <c r="AE32" s="25">
+      <c r="AE32" s="23">
         <v>37</v>
       </c>
-      <c r="AF32" s="25">
+      <c r="AF32" s="60">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AJ5:AO5"/>
+    <mergeCell ref="AJ10:AO10"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="AD1:AF1"/>
     <mergeCell ref="R16:Y16"/>
     <mergeCell ref="R20:Y20"/>
     <mergeCell ref="R6:Y6"/>
     <mergeCell ref="R10:Y10"/>
     <mergeCell ref="R5:Y5"/>
     <mergeCell ref="R15:Y15"/>
-    <mergeCell ref="AJ5:AO5"/>
-    <mergeCell ref="AJ10:AO10"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="AD1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>